<commit_message>
admin login broken in a sudden although no changes have been made in that view.
完成國中部/高中部課程單一選擇的部分
</commit_message>
<xml_diff>
--- a/DBzip/db_import.xlsx
+++ b/DBzip/db_import.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/a10910/Documents/,2025花東音樂營/,course selection system/HTCCCS/DBzip/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB16550F-3696-0945-9A18-C36B5CB43808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DF1864-E9FD-AF46-88A3-067BF49D9992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="80" yWindow="780" windowWidth="34120" windowHeight="19820" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -120,7 +120,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="625" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="319">
   <si>
     <t>section_id</t>
   </si>
@@ -1067,6 +1067,18 @@
   </si>
   <si>
     <t>第十二節</t>
+  </si>
+  <si>
+    <t>hs</t>
+  </si>
+  <si>
+    <t>國中部課程</t>
+  </si>
+  <si>
+    <t>js</t>
+  </si>
+  <si>
+    <t>測試國中部課程</t>
   </si>
 </sst>
 </file>
@@ -4184,10 +4196,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F70"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B73" sqref="B73"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C71" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4828,7 +4840,7 @@
         <v>99</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>226</v>
+        <v>315</v>
       </c>
       <c r="F37" s="2">
         <v>3</v>
@@ -4846,7 +4858,7 @@
         <v>99</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>226</v>
+        <v>315</v>
       </c>
       <c r="F38" s="2">
         <v>5</v>
@@ -5396,6 +5408,23 @@
       </c>
       <c r="F70" s="2">
         <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>316</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>317</v>
+      </c>
+      <c r="F71" s="2">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>